<commit_message>
New datadriven testcases added
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagav\eclipse-workspace\AutomationStepByStep\SeleniumWebDriverManager\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagav\eclipse-workspace\AutomationStepByStep\MagentoSelenium\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02DCD5C-2414-4F97-96A7-37874967EF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D00972F-4B1A-4CA7-9C2B-3BB4BAD76A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34500" yWindow="1860" windowWidth="18045" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34500" yWindow="1860" windowWidth="18045" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -36,9 +37,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>Admin1</t>
   </si>
   <si>
@@ -52,6 +50,24 @@
   </si>
   <si>
     <t>Admin3</t>
+  </si>
+  <si>
+    <t>testadmin123</t>
+  </si>
+  <si>
+    <t>SearchData</t>
+  </si>
+  <si>
+    <t>Bag</t>
+  </si>
+  <si>
+    <t>abab</t>
+  </si>
+  <si>
+    <t>belt</t>
+  </si>
+  <si>
+    <t>Jacket</t>
   </si>
 </sst>
 </file>
@@ -371,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,31 +410,74 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CC3E48-6B8C-4D0B-95AF-D4C5A6995719}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>